<commit_message>
Consistent indent between font and pattern CF formatting toString indent
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1694087 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/Themes.xlsx
+++ b/test-data/spreadsheet/Themes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="11535"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>dk1</t>
   </si>
@@ -50,13 +50,70 @@
   </si>
   <si>
     <t>folhlink</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>Theme Colours</t>
+  </si>
+  <si>
+    <t>Explicit</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Grey</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>std red</t>
+  </si>
+  <si>
+    <t>std green</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,13 +198,113 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC0C0C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -176,17 +333,291 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF0000FF"/>
+      <color rgb="FFC0C0C0"/>
+      <color rgb="FF000000"/>
       <color rgb="FF800080"/>
-      <color rgb="FF0000FF"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -272,7 +703,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -307,7 +737,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -483,77 +912,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="16" customFormat="1">
+      <c r="A1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G3:G5 G7">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5 G7">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"std red"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"std green"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>